<commit_message>
Added a function to clean NIR files and updated 2021 Yield nir files
</commit_message>
<xml_diff>
--- a/sandbox/data/yieldfiles_2021/2021_USB 5 Early_PLY.xlsx
+++ b/sandbox/data/yieldfiles_2021/2021_USB 5 Early_PLY.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soybean\Desktop\2021 Mian\Harvest Info\2021_Yield_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehuie\Nextcloud\MIAN\2021 Mian\Harvest Info\2021_Yield_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A825A-1E1B-401C-A5A5-55ACBA030E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="11091" windowHeight="4277"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USB Oil 5 Early" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="36">
   <si>
     <t>Genotype</t>
   </si>
@@ -109,12 +110,30 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>indet</t>
+  </si>
+  <si>
+    <t>thin</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -917,21 +936,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="91" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.15234375" style="1"/>
-    <col min="3" max="3" width="13.15234375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.15234375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1025,17 @@
       <c r="I2" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1032,8 +1060,20 @@
       <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="I3" s="1">
+        <v>34</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1058,8 +1098,20 @@
       <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="I4" s="1">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1087,8 +1139,17 @@
       <c r="I5" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1116,8 +1177,17 @@
       <c r="I6" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1145,8 +1215,17 @@
       <c r="I7" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1174,8 +1253,20 @@
       <c r="I8" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>48</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1203,8 +1294,17 @@
       <c r="I9" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1232,8 +1332,17 @@
       <c r="I10" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1261,8 +1370,17 @@
       <c r="I11" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1290,8 +1408,17 @@
       <c r="I12" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1319,8 +1446,17 @@
       <c r="I13" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="J13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L13" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1345,8 +1481,20 @@
       <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="I14" s="1">
+        <v>35</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L14" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1371,8 +1519,20 @@
       <c r="H15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="I15" s="1">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1400,8 +1560,17 @@
       <c r="I16" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L16" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1426,8 +1595,20 @@
       <c r="H17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I17" s="1">
+        <v>36</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1455,8 +1636,17 @@
       <c r="I18" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1484,8 +1674,20 @@
       <c r="I19" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>21</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1513,8 +1715,17 @@
       <c r="I20" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L20" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1542,8 +1753,20 @@
       <c r="I21" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>46</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1568,11 +1791,20 @@
       <c r="H22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="K22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1597,11 +1829,20 @@
       <c r="H23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1626,11 +1867,20 @@
       <c r="H24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1655,11 +1905,20 @@
       <c r="H25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1684,11 +1943,20 @@
       <c r="H26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1713,11 +1981,20 @@
       <c r="H27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1742,11 +2019,20 @@
       <c r="H28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1771,11 +2057,20 @@
       <c r="H29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,8 +2095,20 @@
       <c r="H30" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
@@ -1826,12 +2133,24 @@
       <c r="H31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="1">
-        <v>30</v>
+      <c r="I31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P31">
     <sortCondition ref="G2:G31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>